<commit_message>
update group work assignment sheet
</commit_message>
<xml_diff>
--- a/Documents/Group Work Assignment.xlsx
+++ b/Documents/Group Work Assignment.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Group Member</t>
   </si>
@@ -70,6 +70,9 @@
     <t>3. Interface prototype</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/0BwilqVT1NDYIV0RrbG1HLWRoVmM/view?usp=sharing</t>
+  </si>
+  <si>
     <t>Di Wang</t>
   </si>
   <si>
@@ -82,6 +85,9 @@
     <t>2. Paper prototype</t>
   </si>
   <si>
+    <t>https://drive.google.com/drive/folders/0B6lY9JarSd33RUlrdFNtMENya1k</t>
+  </si>
+  <si>
     <t>3. Test tasks -- Testing round1</t>
   </si>
   <si>
@@ -92,13 +98,61 @@
   </si>
   <si>
     <t>1. Wireframe -- Interface (profile &amp; owner )</t>
+  </si>
+  <si>
+    <t>Week 11 &amp; Week 12</t>
+  </si>
+  <si>
+    <t>1. Community Page Front-end</t>
+  </si>
+  <si>
+    <t>joblist-care.html/grouplist-care.html</t>
+  </si>
+  <si>
+    <t>2. Me Page Front-end</t>
+  </si>
+  <si>
+    <t>group-chat.html</t>
+  </si>
+  <si>
+    <t>3. Detail Pages</t>
+  </si>
+  <si>
+    <t>within group-chat.html grouplist-care.html</t>
+  </si>
+  <si>
+    <t>1. Test Wireframe</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=0B6lY9JarSd33SGYwRzF2U1J6ZU0</t>
+  </si>
+  <si>
+    <t>2. Design Alternative</t>
+  </si>
+  <si>
+    <t>1. Community Page Share/ Apply</t>
+  </si>
+  <si>
+    <t>joblist_care.html/grouplist_care.html</t>
+  </si>
+  <si>
+    <t>2. Me Page Vote/ Task check</t>
+  </si>
+  <si>
+    <t>group_chat.html</t>
+  </si>
+  <si>
+    <t>Di Wany</t>
+  </si>
+  <si>
+    <t>1. Final Document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -127,11 +181,15 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,12 +204,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border/>
     <border>
       <right style="thin">
@@ -184,51 +248,76 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,9 +333,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -392,7 +478,7 @@
       <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -446,7 +532,9 @@
       <c r="C9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -472,34 +560,36 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -526,25 +616,27 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -568,31 +660,125 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
+    <row r="15">
+      <c r="A15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="16">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17">
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18">
-      <c r="C18" s="14"/>
+      <c r="A18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="19"/>
     </row>
     <row r="20">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21">
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22">
-      <c r="C22" s="14"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -602,10 +788,15 @@
     <hyperlink r:id="rId4" ref="D5"/>
     <hyperlink r:id="rId5" ref="D7"/>
     <hyperlink r:id="rId6" ref="D8"/>
-    <hyperlink r:id="rId7" ref="D10"/>
-    <hyperlink r:id="rId8" ref="D12"/>
-    <hyperlink r:id="rId9" ref="D13"/>
+    <hyperlink r:id="rId7" ref="D9"/>
+    <hyperlink r:id="rId8" ref="D10"/>
+    <hyperlink r:id="rId9" ref="D11"/>
+    <hyperlink r:id="rId10" ref="D12"/>
+    <hyperlink r:id="rId11" ref="D13"/>
+    <hyperlink r:id="rId12" ref="D14"/>
+    <hyperlink r:id="rId13" ref="D18"/>
+    <hyperlink r:id="rId14" ref="D22"/>
   </hyperlinks>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>